<commit_message>
Scenario: Wryonin vs Mudrich 1v1
</commit_message>
<xml_diff>
--- a/Test/test_runs_combat.xlsx
+++ b/Test/test_runs_combat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shield\Documents\Story\AgranariTTRPG\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0178F633-74C2-4BD9-A3FB-605139EE2A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349EA99A-8BF4-4484-8EDF-B5BBB194BA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12975" yWindow="405" windowWidth="29070" windowHeight="12600" xr2:uid="{F8D463A0-768A-4A18-944B-E333205F072A}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="122">
   <si>
     <t>Cat Soldier</t>
   </si>
@@ -426,6 +426,9 @@
   <si>
     <t>CRIT!</t>
   </si>
+  <si>
+    <t>Elbow</t>
+  </si>
 </sst>
 </file>
 
@@ -752,7 +755,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FFBFBFBF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFBFBFBF"/>
@@ -1154,10 +1167,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7A2475-8FD1-4D1A-98B6-D7C93564AF9C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y779"/>
+  <dimension ref="A1:Y807"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A674" workbookViewId="0">
-      <selection activeCell="L688" sqref="L688"/>
+    <sheetView tabSelected="1" topLeftCell="A785" workbookViewId="0">
+      <selection activeCell="A790" sqref="A790:X807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22095,6 +22108,816 @@
       <c r="W779" s="27"/>
       <c r="X779" s="32"/>
     </row>
+    <row r="790" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A790" s="27"/>
+      <c r="B790" s="27"/>
+      <c r="C790" s="27"/>
+      <c r="D790" s="27"/>
+      <c r="E790" s="27"/>
+      <c r="F790" s="27"/>
+      <c r="G790" s="27"/>
+      <c r="H790" s="27"/>
+      <c r="I790" s="27"/>
+      <c r="J790" s="27"/>
+      <c r="K790" s="27"/>
+      <c r="L790" s="27"/>
+      <c r="M790" s="27"/>
+      <c r="N790" s="27"/>
+      <c r="O790" s="27"/>
+      <c r="P790" s="27"/>
+      <c r="Q790" s="27"/>
+      <c r="R790" s="27"/>
+      <c r="S790" s="27"/>
+      <c r="T790" s="27"/>
+      <c r="U790" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="V790" s="28"/>
+      <c r="W790" s="28"/>
+      <c r="X790" s="28"/>
+    </row>
+    <row r="791" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A791" s="29"/>
+      <c r="B791" s="29"/>
+      <c r="C791" s="29"/>
+      <c r="D791" s="29"/>
+      <c r="E791" s="29"/>
+      <c r="F791" s="29"/>
+      <c r="G791" s="29"/>
+      <c r="H791" s="29"/>
+      <c r="I791" s="29"/>
+      <c r="J791" s="29"/>
+      <c r="K791" s="29"/>
+      <c r="L791" s="27"/>
+      <c r="M791" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="N791" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="O791" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="P791" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q791" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="R791" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="S791" s="27"/>
+      <c r="T791" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="U791" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="V791" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="W791" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="X791" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="792" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A792" s="29"/>
+      <c r="B792" s="29"/>
+      <c r="C792" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D792" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E792" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F792" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G792" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="H792" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I792" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J792" s="29"/>
+      <c r="K792" s="29"/>
+      <c r="L792" s="27"/>
+      <c r="M792" s="49">
+        <v>1</v>
+      </c>
+      <c r="N792" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O792" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="P792" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q792" s="33">
+        <v>1</v>
+      </c>
+      <c r="R792" s="33">
+        <v>1</v>
+      </c>
+      <c r="S792" s="27"/>
+      <c r="T792" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="U792" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="V792" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="W792" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="X792" s="32">
+        <v>4.4159660180409759</v>
+      </c>
+    </row>
+    <row r="793" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A793" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B793" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C793" s="36">
+        <v>7.7272727272727275</v>
+      </c>
+      <c r="D793" s="37"/>
+      <c r="E793" s="36">
+        <v>26.453222831090294</v>
+      </c>
+      <c r="F793" s="44"/>
+      <c r="G793" s="36">
+        <v>0</v>
+      </c>
+      <c r="H793" s="36">
+        <v>1</v>
+      </c>
+      <c r="I793" s="38">
+        <v>34.18049555836302</v>
+      </c>
+      <c r="J793" s="39"/>
+      <c r="K793" s="29"/>
+      <c r="L793" s="27"/>
+      <c r="M793" s="49">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N793" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="O793" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P793" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q793" s="33">
+        <v>11</v>
+      </c>
+      <c r="R793" s="33">
+        <v>1</v>
+      </c>
+      <c r="S793" s="27"/>
+      <c r="T793" s="27"/>
+      <c r="U793" s="27"/>
+      <c r="V793" s="27"/>
+      <c r="W793" s="27"/>
+      <c r="X793" s="32"/>
+    </row>
+    <row r="794" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A794" s="29"/>
+      <c r="B794" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C794" s="36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D794" s="37"/>
+      <c r="E794" s="36"/>
+      <c r="F794" s="44"/>
+      <c r="G794" s="36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H794" s="36">
+        <v>1</v>
+      </c>
+      <c r="I794" s="38" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J794" s="39"/>
+      <c r="K794" s="29"/>
+      <c r="L794" s="27"/>
+      <c r="M794" s="49">
+        <v>2</v>
+      </c>
+      <c r="N794" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="O794" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P794" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q794" s="33">
+        <v>2</v>
+      </c>
+      <c r="R794" s="33">
+        <v>2</v>
+      </c>
+      <c r="S794" s="27"/>
+      <c r="T794" s="27">
+        <v>0</v>
+      </c>
+      <c r="U794" s="27"/>
+      <c r="V794" s="27"/>
+      <c r="W794" s="27"/>
+      <c r="X794" s="32"/>
+    </row>
+    <row r="795" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A795" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B795" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C795" s="36">
+        <v>0.8</v>
+      </c>
+      <c r="D795" s="37"/>
+      <c r="E795" s="36">
+        <v>30.866805553436279</v>
+      </c>
+      <c r="F795" s="44"/>
+      <c r="G795" s="36">
+        <v>0</v>
+      </c>
+      <c r="H795" s="36">
+        <v>1</v>
+      </c>
+      <c r="I795" s="38">
+        <v>31.66680555343628</v>
+      </c>
+      <c r="J795" s="39"/>
+      <c r="K795" s="29"/>
+      <c r="L795" s="27"/>
+      <c r="M795" s="49">
+        <v>3</v>
+      </c>
+      <c r="N795" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O795" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="P795" s="32">
+        <v>34.182987610499062</v>
+      </c>
+      <c r="Q795" s="33">
+        <v>1</v>
+      </c>
+      <c r="R795" s="33">
+        <v>13</v>
+      </c>
+      <c r="S795" s="27"/>
+      <c r="T795" s="27"/>
+      <c r="U795" s="27"/>
+      <c r="V795" s="27"/>
+      <c r="W795" s="27"/>
+      <c r="X795" s="32"/>
+    </row>
+    <row r="796" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A796" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B796" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C796" s="36">
+        <v>50</v>
+      </c>
+      <c r="D796" s="37"/>
+      <c r="E796" s="36">
+        <v>2.6082723140716553</v>
+      </c>
+      <c r="F796" s="44"/>
+      <c r="G796" s="36">
+        <v>0</v>
+      </c>
+      <c r="H796" s="36">
+        <v>1</v>
+      </c>
+      <c r="I796" s="38">
+        <v>52.608272314071655</v>
+      </c>
+      <c r="J796" s="39"/>
+      <c r="K796" s="29"/>
+      <c r="L796" s="27"/>
+      <c r="M796" s="49">
+        <v>4</v>
+      </c>
+      <c r="N796" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="O796" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P796" s="32">
+        <v>51.062067846457168</v>
+      </c>
+      <c r="Q796" s="33">
+        <v>1</v>
+      </c>
+      <c r="R796" s="33">
+        <v>22</v>
+      </c>
+      <c r="S796" s="27"/>
+      <c r="T796" s="27"/>
+      <c r="U796" s="27"/>
+      <c r="V796" s="27"/>
+      <c r="W796" s="27"/>
+      <c r="X796" s="32"/>
+    </row>
+    <row r="797" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A797" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B797" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C797" s="36"/>
+      <c r="D797" s="36"/>
+      <c r="E797" s="36"/>
+      <c r="F797" s="45"/>
+      <c r="G797" s="36">
+        <v>0</v>
+      </c>
+      <c r="H797" s="36">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I797" s="40">
+        <v>43.840226928393051</v>
+      </c>
+      <c r="J797" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="K797" s="29"/>
+      <c r="L797" s="27"/>
+      <c r="M797" s="49">
+        <v>5</v>
+      </c>
+      <c r="N797" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="O797" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P797" s="32">
+        <v>51.148905555407211</v>
+      </c>
+      <c r="Q797" s="33">
+        <v>0</v>
+      </c>
+      <c r="R797" s="33">
+        <v>1</v>
+      </c>
+      <c r="S797" s="27"/>
+      <c r="T797" s="27"/>
+      <c r="U797" s="27"/>
+      <c r="V797" s="27"/>
+      <c r="W797" s="27"/>
+      <c r="X797" s="32"/>
+    </row>
+    <row r="798" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A798" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B798" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C798" s="36">
+        <v>24.983333333333334</v>
+      </c>
+      <c r="D798" s="37"/>
+      <c r="E798" s="36">
+        <v>14.440927577018739</v>
+      </c>
+      <c r="F798" s="44"/>
+      <c r="G798" s="36">
+        <v>0</v>
+      </c>
+      <c r="H798" s="36">
+        <v>1</v>
+      </c>
+      <c r="I798" s="38">
+        <v>39.424260910352075</v>
+      </c>
+      <c r="J798" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="K798" s="29"/>
+      <c r="L798" s="27"/>
+      <c r="M798" s="49">
+        <v>6</v>
+      </c>
+      <c r="N798" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="O798" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P798" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q798" s="33">
+        <v>0</v>
+      </c>
+      <c r="R798" s="33">
+        <v>0</v>
+      </c>
+      <c r="S798" s="27"/>
+      <c r="T798" s="27"/>
+      <c r="U798" s="27"/>
+      <c r="V798" s="27"/>
+      <c r="W798" s="27"/>
+      <c r="X798" s="32"/>
+    </row>
+    <row r="799" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A799" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B799" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C799" s="36">
+        <v>13.893181818181819</v>
+      </c>
+      <c r="D799" s="37"/>
+      <c r="E799" s="36">
+        <v>8.1309923484921462</v>
+      </c>
+      <c r="F799" s="44"/>
+      <c r="G799" s="36">
+        <v>0</v>
+      </c>
+      <c r="H799" s="36">
+        <v>1</v>
+      </c>
+      <c r="I799" s="38">
+        <v>22.024174166673966</v>
+      </c>
+      <c r="J799" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="K799" s="29"/>
+      <c r="L799" s="27"/>
+      <c r="M799" s="49">
+        <v>7</v>
+      </c>
+      <c r="N799" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O799" s="27"/>
+      <c r="P799" s="32"/>
+      <c r="Q799" s="33"/>
+      <c r="R799" s="33"/>
+      <c r="S799" s="27"/>
+      <c r="T799" s="27"/>
+      <c r="U799" s="27"/>
+      <c r="V799" s="27"/>
+      <c r="W799" s="27"/>
+      <c r="X799" s="32"/>
+    </row>
+    <row r="800" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A800" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B800" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C800" s="36">
+        <v>123.75</v>
+      </c>
+      <c r="D800" s="37"/>
+      <c r="E800" s="36">
+        <v>6.4162985622882847</v>
+      </c>
+      <c r="F800" s="44"/>
+      <c r="G800" s="36">
+        <v>0</v>
+      </c>
+      <c r="H800" s="36">
+        <v>1</v>
+      </c>
+      <c r="I800" s="38">
+        <v>130.16629856228829</v>
+      </c>
+      <c r="J800" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="K800" s="29"/>
+      <c r="L800" s="27"/>
+      <c r="M800" s="49">
+        <v>7.1</v>
+      </c>
+      <c r="N800" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="O800" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P800" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q800" s="33">
+        <v>0</v>
+      </c>
+      <c r="R800" s="33">
+        <v>0</v>
+      </c>
+      <c r="S800" s="27"/>
+      <c r="T800" s="27"/>
+      <c r="U800" s="27"/>
+      <c r="V800" s="27"/>
+      <c r="W800" s="27"/>
+      <c r="X800" s="32"/>
+    </row>
+    <row r="801" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A801" s="29"/>
+      <c r="B801" s="29"/>
+      <c r="C801" s="29"/>
+      <c r="D801" s="29"/>
+      <c r="E801" s="29"/>
+      <c r="F801" s="29"/>
+      <c r="G801" s="29"/>
+      <c r="H801" s="29"/>
+      <c r="I801" s="29"/>
+      <c r="J801" s="29"/>
+      <c r="K801" s="29"/>
+      <c r="L801" s="27"/>
+      <c r="M801" s="49">
+        <v>8</v>
+      </c>
+      <c r="N801" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O801" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="P801" s="32">
+        <v>38.284235397974648</v>
+      </c>
+      <c r="Q801" s="33">
+        <v>0</v>
+      </c>
+      <c r="R801" s="33">
+        <v>0</v>
+      </c>
+      <c r="S801" s="27"/>
+      <c r="T801" s="27"/>
+      <c r="U801" s="27"/>
+      <c r="V801" s="27"/>
+      <c r="W801" s="27"/>
+      <c r="X801" s="32"/>
+    </row>
+    <row r="802" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A802" s="27"/>
+      <c r="B802" s="27"/>
+      <c r="C802" s="27"/>
+      <c r="D802" s="27"/>
+      <c r="E802" s="27"/>
+      <c r="F802" s="27"/>
+      <c r="G802" s="27"/>
+      <c r="H802" s="27"/>
+      <c r="I802" s="27"/>
+      <c r="J802" s="27"/>
+      <c r="K802" s="27"/>
+      <c r="L802" s="27"/>
+      <c r="M802" s="49">
+        <v>9</v>
+      </c>
+      <c r="N802" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="O802" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P802" s="32">
+        <v>43.840226928393051</v>
+      </c>
+      <c r="Q802" s="33">
+        <v>0</v>
+      </c>
+      <c r="R802" s="33">
+        <v>0</v>
+      </c>
+      <c r="S802" s="27"/>
+      <c r="T802" s="27"/>
+      <c r="U802" s="27"/>
+      <c r="V802" s="27"/>
+      <c r="W802" s="27"/>
+      <c r="X802" s="32"/>
+    </row>
+    <row r="803" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A803" s="27"/>
+      <c r="B803" s="27"/>
+      <c r="C803" s="27"/>
+      <c r="D803" s="27"/>
+      <c r="E803" s="27"/>
+      <c r="F803" s="27"/>
+      <c r="G803" s="27"/>
+      <c r="H803" s="27"/>
+      <c r="I803" s="27"/>
+      <c r="J803" s="27"/>
+      <c r="K803" s="27"/>
+      <c r="L803" s="27"/>
+      <c r="M803" s="49"/>
+      <c r="N803" s="27"/>
+      <c r="O803" s="27"/>
+      <c r="P803" s="32"/>
+      <c r="Q803" s="33"/>
+      <c r="R803" s="33"/>
+      <c r="S803" s="27"/>
+      <c r="T803" s="27"/>
+      <c r="U803" s="27"/>
+      <c r="V803" s="27"/>
+      <c r="W803" s="27"/>
+      <c r="X803" s="32"/>
+    </row>
+    <row r="804" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A804" s="27"/>
+      <c r="B804" s="27"/>
+      <c r="C804" s="27"/>
+      <c r="D804" s="27"/>
+      <c r="E804" s="27"/>
+      <c r="F804" s="27"/>
+      <c r="G804" s="27"/>
+      <c r="H804" s="27"/>
+      <c r="I804" s="27"/>
+      <c r="J804" s="27"/>
+      <c r="K804" s="27"/>
+      <c r="L804" s="27"/>
+      <c r="M804" s="49"/>
+      <c r="N804" s="27"/>
+      <c r="O804" s="27"/>
+      <c r="P804" s="32"/>
+      <c r="Q804" s="33"/>
+      <c r="R804" s="33"/>
+      <c r="S804" s="27"/>
+      <c r="T804" s="27"/>
+      <c r="U804" s="27"/>
+      <c r="V804" s="27"/>
+      <c r="W804" s="27"/>
+      <c r="X804" s="32"/>
+    </row>
+    <row r="805" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A805" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B805" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C805" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D805" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E805" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F805" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G805" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H805" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I805" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="J805" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="K805" s="28"/>
+      <c r="L805" s="28"/>
+      <c r="M805" s="49"/>
+      <c r="N805" s="27"/>
+      <c r="O805" s="27"/>
+      <c r="P805" s="32"/>
+      <c r="Q805" s="33"/>
+      <c r="R805" s="33"/>
+      <c r="S805" s="27"/>
+      <c r="T805" s="27"/>
+      <c r="U805" s="27"/>
+      <c r="V805" s="27"/>
+      <c r="W805" s="27"/>
+      <c r="X805" s="32"/>
+    </row>
+    <row r="806" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A806" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B806" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C806" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D806" s="32">
+        <v>16</v>
+      </c>
+      <c r="E806" s="32">
+        <v>95.448799669742584</v>
+      </c>
+      <c r="F806" s="32">
+        <v>241.5</v>
+      </c>
+      <c r="G806" s="32">
+        <v>0.66666666666666785</v>
+      </c>
+      <c r="H806" s="32">
+        <v>28.666666666666668</v>
+      </c>
+      <c r="I806" s="32"/>
+      <c r="J806" s="27">
+        <v>0</v>
+      </c>
+      <c r="K806" s="27"/>
+      <c r="L806" s="27"/>
+      <c r="M806" s="49"/>
+      <c r="N806" s="27"/>
+      <c r="O806" s="27"/>
+      <c r="P806" s="32"/>
+      <c r="Q806" s="33"/>
+      <c r="R806" s="33"/>
+      <c r="S806" s="27"/>
+      <c r="T806" s="27"/>
+      <c r="U806" s="27"/>
+      <c r="V806" s="27"/>
+      <c r="W806" s="27"/>
+      <c r="X806" s="32"/>
+    </row>
+    <row r="807" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A807" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B807" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C807" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D807" s="32">
+        <v>16</v>
+      </c>
+      <c r="E807" s="32">
+        <v>167.5327769915263</v>
+      </c>
+      <c r="F807" s="32">
+        <v>240</v>
+      </c>
+      <c r="G807" s="32">
+        <v>0</v>
+      </c>
+      <c r="H807" s="32">
+        <v>28</v>
+      </c>
+      <c r="I807" s="32"/>
+      <c r="J807" s="32">
+        <v>0</v>
+      </c>
+      <c r="K807" s="32"/>
+      <c r="L807" s="32"/>
+      <c r="M807" s="49"/>
+      <c r="N807" s="27"/>
+      <c r="O807" s="27"/>
+      <c r="P807" s="32"/>
+      <c r="Q807" s="33"/>
+      <c r="R807" s="33"/>
+      <c r="S807" s="27"/>
+      <c r="T807" s="27"/>
+      <c r="U807" s="27"/>
+      <c r="V807" s="27"/>
+      <c r="W807" s="27"/>
+      <c r="X807" s="32"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="G197:I197"/>
@@ -22109,6 +22932,16 @@
     <mergeCell ref="V190:W190"/>
   </mergeCells>
   <conditionalFormatting sqref="E367:F375">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF7C7AC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E467:F475">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -22118,7 +22951,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E467:F475">
+  <conditionalFormatting sqref="E547:F555">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -22128,7 +22961,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E547:F555">
+  <conditionalFormatting sqref="E588:F595">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -22138,7 +22971,57 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E588:F595">
+  <conditionalFormatting sqref="G366:H375">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFA6C9EC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G466:H475">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFA6C9EC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G546:H555">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFA6C9EC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G586:H595">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFA6C9EC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G693:H702">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFA6C9EC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E695:F702">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -22148,8 +23031,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G366:H375">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="P677:R779">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G806:H807">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -22158,63 +23046,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G466:H475">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFA6C9EC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G546:H555">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFA6C9EC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G586:H595">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFA6C9EC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G693:H702">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFA6C9EC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E695:F702">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFF7C7AC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P677:R779">
+  <conditionalFormatting sqref="P790:R807">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L299:M332 S352:S430 M352:N430 U452:U525 O452:P525 O532:P569 U532:U569 T572:T671 N572:O671 T682:T779 T679:T680 N679:O779" xr:uid="{804F0AFC-E07C-4B9B-A3FD-AEB68EC6AC1C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L299:M332 S352:S430 M352:N430 U452:U525 O452:P525 O532:P569 U532:U569 T572:T671 N572:O671 T682:T779 T679:T680 N679:O779 T795:T807 T792:T793 N792:O807" xr:uid="{804F0AFC-E07C-4B9B-A3FD-AEB68EC6AC1C}">
       <formula1>$A$18:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B208:C208" xr:uid="{605C8630-B0BC-4DB7-8E8F-8A6B69239C15}">

</xml_diff>